<commit_message>
Clase 4 CSS Avanzado
</commit_message>
<xml_diff>
--- a/clase4/GridComponents.xlsx
+++ b/clase4/GridComponents.xlsx
@@ -258,9 +258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -278,22 +275,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -309,21 +294,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -340,6 +316,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -638,48 +638,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="2:16">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="F2" s="74" t="s">
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="F2" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="K2" s="75" t="s">
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="K2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
     </row>
     <row r="3" spans="2:16" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:16">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="41" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="F4" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="D4" s="42"/>
+      <c r="F4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="27" t="s">
         <v>4</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -694,17 +694,17 @@
       <c r="P4" s="3"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
       <c r="K5" s="4"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -713,15 +713,15 @@
       <c r="P5" s="6"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="45"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="46" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="32"/>
+      <c r="D6" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="28"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="31"/>
       <c r="K6" s="4"/>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
@@ -732,17 +732,17 @@
       </c>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="32"/>
+      <c r="B7" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="72"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="69"/>
+      <c r="I7" s="31"/>
       <c r="K7" s="4"/>
       <c r="L7" s="10" t="s">
         <v>3</v>
@@ -755,17 +755,17 @@
       <c r="P7" s="9"/>
     </row>
     <row r="8" spans="2:16">
-      <c r="B8" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="51" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="52"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="35"/>
+      <c r="B8" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="34"/>
       <c r="K8" s="4"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -776,17 +776,17 @@
       </c>
     </row>
     <row r="9" spans="2:16">
-      <c r="B9" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="55"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="35"/>
+      <c r="B9" s="48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="34"/>
       <c r="K9" s="4"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -795,13 +795,13 @@
       <c r="P9" s="12"/>
     </row>
     <row r="10" spans="2:16">
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="35"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="34"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5" t="s">
         <v>3</v>
@@ -812,19 +812,19 @@
       <c r="P10" s="6"/>
     </row>
     <row r="11" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="51" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="39"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="41" t="s">
+      <c r="F11" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="40" t="s">
         <v>4</v>
       </c>
       <c r="K11" s="14"/>
@@ -835,48 +835,48 @@
       <c r="P11" s="16"/>
     </row>
     <row r="12" spans="2:16">
-      <c r="B12" s="56"/>
+      <c r="B12" s="51"/>
       <c r="C12" s="10"/>
       <c r="D12" s="12"/>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="67"/>
+      <c r="B13" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="74"/>
+      <c r="D13" s="75"/>
     </row>
     <row r="14" spans="2:16">
-      <c r="B14" s="57"/>
+      <c r="B14" s="52"/>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="2:16">
-      <c r="B15" s="69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="70"/>
-      <c r="K15" s="75" t="s">
+      <c r="B15" s="60" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="62"/>
+      <c r="K15" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="L15" s="75"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="75"/>
-      <c r="P15" s="75"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
     </row>
     <row r="16" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B16" s="57"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
     </row>
     <row r="17" spans="2:16">
-      <c r="B17" s="71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="72"/>
-      <c r="D17" s="73"/>
+      <c r="B17" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
       <c r="K17" s="1" t="s">
         <v>3</v>
       </c>
@@ -891,13 +891,13 @@
       <c r="P17" s="18"/>
     </row>
     <row r="18" spans="2:16">
-      <c r="B18" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="58" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="59"/>
+      <c r="B18" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="54"/>
       <c r="K18" s="4"/>
       <c r="L18" s="5"/>
       <c r="M18" s="13"/>
@@ -908,9 +908,9 @@
       </c>
     </row>
     <row r="19" spans="2:16">
-      <c r="B19" s="45"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="59"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="54"/>
       <c r="K19" s="4"/>
       <c r="L19" s="5"/>
       <c r="M19" s="20"/>
@@ -919,7 +919,7 @@
       <c r="P19" s="19"/>
     </row>
     <row r="20" spans="2:16">
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="8" t="s">
@@ -936,13 +936,13 @@
       <c r="P20" s="19"/>
     </row>
     <row r="21" spans="2:16">
-      <c r="B21" s="61" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="52"/>
+      <c r="B21" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="47"/>
       <c r="K21" s="4"/>
       <c r="L21" s="5"/>
       <c r="M21" s="10"/>
@@ -953,9 +953,9 @@
       <c r="P21" s="19"/>
     </row>
     <row r="22" spans="2:16">
-      <c r="B22" s="61"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
       <c r="K22" s="4"/>
       <c r="L22" s="5"/>
       <c r="M22" s="21"/>
@@ -964,9 +964,9 @@
       <c r="P22" s="19"/>
     </row>
     <row r="23" spans="2:16">
-      <c r="B23" s="61"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
       <c r="K23" s="4"/>
       <c r="L23" s="5"/>
       <c r="M23" s="13" t="s">
@@ -977,11 +977,11 @@
       <c r="P23" s="19"/>
     </row>
     <row r="24" spans="2:16" ht="15.75" thickBot="1">
-      <c r="B24" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="64" t="s">
+      <c r="B24" s="57" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="58"/>
+      <c r="D24" s="59" t="s">
         <v>4</v>
       </c>
       <c r="K24" s="14"/>

</xml_diff>